<commit_message>
Update harrington functions in test.py
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1071,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>20</v>
@@ -1091,7 +1091,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>20</v>
@@ -1111,7 +1111,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -1131,7 +1131,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -1151,7 +1151,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>

</xml_diff>